<commit_message>
Region/Station info now pulls from CCPs data dump
Updated the station/region ID swaps to pull from Eves official data dumps and not an excel file.
</commit_message>
<xml_diff>
--- a/data/outputs/Market_Sell_Data.xlsx
+++ b/data/outputs/Market_Sell_Data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="64">
   <si>
     <t>Item</t>
   </si>
@@ -206,7 +206,7 @@
     <t>Certh Finley</t>
   </si>
   <si>
-    <t>06/25/2023, 16:11:45</t>
+    <t>06/26/2023, 13:41:20</t>
   </si>
 </sst>
 </file>
@@ -564,7 +564,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E144"/>
+  <dimension ref="A1:E142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -601,7 +601,7 @@
         <v>133400</v>
       </c>
       <c r="E2">
-        <v>5136</v>
+        <v>4969</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -632,10 +632,10 @@
         <v>55</v>
       </c>
       <c r="D4">
-        <v>134400</v>
+        <v>142500</v>
       </c>
       <c r="E4">
-        <v>216</v>
+        <v>6495</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -683,10 +683,10 @@
         <v>53</v>
       </c>
       <c r="D7">
-        <v>40070</v>
+        <v>39850</v>
       </c>
       <c r="E7">
-        <v>3300</v>
+        <v>54546</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -703,7 +703,7 @@
         <v>41870</v>
       </c>
       <c r="E8">
-        <v>10000</v>
+        <v>9392</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -717,10 +717,10 @@
         <v>53</v>
       </c>
       <c r="D9">
-        <v>39700</v>
+        <v>34480</v>
       </c>
       <c r="E9">
-        <v>3041</v>
+        <v>9571</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -754,7 +754,7 @@
         <v>41970</v>
       </c>
       <c r="E11">
-        <v>5000</v>
+        <v>4644</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -771,7 +771,7 @@
         <v>58740</v>
       </c>
       <c r="E12">
-        <v>25418</v>
+        <v>24689</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -788,7 +788,7 @@
         <v>26640</v>
       </c>
       <c r="E13">
-        <v>12139</v>
+        <v>6680</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -836,10 +836,10 @@
         <v>53</v>
       </c>
       <c r="D16">
-        <v>66740</v>
+        <v>65310</v>
       </c>
       <c r="E16">
-        <v>5171</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -887,10 +887,10 @@
         <v>53</v>
       </c>
       <c r="D19">
-        <v>11950</v>
+        <v>11490</v>
       </c>
       <c r="E19">
-        <v>24000</v>
+        <v>21250</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -907,7 +907,7 @@
         <v>27000</v>
       </c>
       <c r="E20">
-        <v>25950</v>
+        <v>25650</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -921,10 +921,10 @@
         <v>55</v>
       </c>
       <c r="D21">
-        <v>24000</v>
+        <v>23320</v>
       </c>
       <c r="E21">
-        <v>126000</v>
+        <v>74245</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -955,10 +955,10 @@
         <v>53</v>
       </c>
       <c r="D23">
-        <v>222</v>
+        <v>218.5</v>
       </c>
       <c r="E23">
-        <v>17080280</v>
+        <v>4233973</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1040,10 +1040,10 @@
         <v>53</v>
       </c>
       <c r="D28">
-        <v>17320</v>
+        <v>17100</v>
       </c>
       <c r="E28">
-        <v>55470</v>
+        <v>214722</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1074,10 +1074,10 @@
         <v>55</v>
       </c>
       <c r="D30">
-        <v>22720</v>
+        <v>22670</v>
       </c>
       <c r="E30">
-        <v>64100</v>
+        <v>59100</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1094,7 +1094,7 @@
         <v>179600</v>
       </c>
       <c r="E31">
-        <v>10191</v>
+        <v>9782</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1125,10 +1125,10 @@
         <v>55</v>
       </c>
       <c r="D33">
-        <v>104400</v>
+        <v>104500</v>
       </c>
       <c r="E33">
-        <v>651</v>
+        <v>2164</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1142,10 +1142,10 @@
         <v>53</v>
       </c>
       <c r="D34">
-        <v>42410</v>
+        <v>42450</v>
       </c>
       <c r="E34">
-        <v>2805</v>
+        <v>19999</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1176,10 +1176,10 @@
         <v>55</v>
       </c>
       <c r="D36">
-        <v>51820</v>
+        <v>51790</v>
       </c>
       <c r="E36">
-        <v>2050</v>
+        <v>2634</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1193,10 +1193,10 @@
         <v>53</v>
       </c>
       <c r="D37">
-        <v>37470</v>
+        <v>37220</v>
       </c>
       <c r="E37">
-        <v>71423</v>
+        <v>70923</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1230,7 +1230,7 @@
         <v>38950</v>
       </c>
       <c r="E39">
-        <v>5000</v>
+        <v>6679</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1247,7 +1247,7 @@
         <v>19720</v>
       </c>
       <c r="E40">
-        <v>107746</v>
+        <v>101971</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1332,7 +1332,7 @@
         <v>55670</v>
       </c>
       <c r="E45">
-        <v>43836</v>
+        <v>34609</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1363,10 +1363,10 @@
         <v>53</v>
       </c>
       <c r="D47">
-        <v>11480</v>
+        <v>11430</v>
       </c>
       <c r="E47">
-        <v>22787</v>
+        <v>21725</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1397,10 +1397,10 @@
         <v>55</v>
       </c>
       <c r="D49">
-        <v>27000</v>
+        <v>26870</v>
       </c>
       <c r="E49">
-        <v>68856</v>
+        <v>163730</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1414,10 +1414,10 @@
         <v>53</v>
       </c>
       <c r="D50">
-        <v>169.3</v>
+        <v>169.5</v>
       </c>
       <c r="E50">
-        <v>5661830</v>
+        <v>3683907</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1434,7 +1434,7 @@
         <v>213.6</v>
       </c>
       <c r="E51">
-        <v>1700805</v>
+        <v>1660805</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1448,10 +1448,10 @@
         <v>55</v>
       </c>
       <c r="D52">
-        <v>188</v>
+        <v>209.8</v>
       </c>
       <c r="E52">
-        <v>2360000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1499,10 +1499,10 @@
         <v>53</v>
       </c>
       <c r="D55">
-        <v>16690</v>
+        <v>16550</v>
       </c>
       <c r="E55">
-        <v>100134</v>
+        <v>197452</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1536,7 +1536,7 @@
         <v>40430</v>
       </c>
       <c r="E57">
-        <v>12552</v>
+        <v>5534</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1570,7 +1570,7 @@
         <v>48380</v>
       </c>
       <c r="E59">
-        <v>3316</v>
+        <v>4665</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1584,10 +1584,10 @@
         <v>53</v>
       </c>
       <c r="D60">
-        <v>49340</v>
+        <v>45000</v>
       </c>
       <c r="E60">
-        <v>10145</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1618,10 +1618,10 @@
         <v>53</v>
       </c>
       <c r="D62">
-        <v>10780</v>
+        <v>10450</v>
       </c>
       <c r="E62">
-        <v>49127</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1638,7 +1638,7 @@
         <v>19200</v>
       </c>
       <c r="E63">
-        <v>62500</v>
+        <v>61145</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1652,10 +1652,10 @@
         <v>55</v>
       </c>
       <c r="D64">
-        <v>18000</v>
+        <v>17960</v>
       </c>
       <c r="E64">
-        <v>62500</v>
+        <v>88271</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1669,10 +1669,10 @@
         <v>57</v>
       </c>
       <c r="D65">
-        <v>19200</v>
+        <v>19180</v>
       </c>
       <c r="E65">
-        <v>62500</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1689,7 +1689,7 @@
         <v>19280</v>
       </c>
       <c r="E66">
-        <v>12863</v>
+        <v>9004</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1720,10 +1720,10 @@
         <v>53</v>
       </c>
       <c r="D68">
-        <v>38800</v>
+        <v>38780</v>
       </c>
       <c r="E68">
-        <v>3007</v>
+        <v>22365</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1737,10 +1737,10 @@
         <v>54</v>
       </c>
       <c r="D69">
-        <v>42900</v>
+        <v>41960</v>
       </c>
       <c r="E69">
-        <v>4477</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1754,7 +1754,7 @@
         <v>55</v>
       </c>
       <c r="D70">
-        <v>49410</v>
+        <v>49240</v>
       </c>
       <c r="E70">
         <v>6917</v>
@@ -1771,10 +1771,10 @@
         <v>53</v>
       </c>
       <c r="D71">
-        <v>98900</v>
+        <v>98910</v>
       </c>
       <c r="E71">
-        <v>727</v>
+        <v>6127</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -1825,7 +1825,7 @@
         <v>34470</v>
       </c>
       <c r="E74">
-        <v>23864</v>
+        <v>14243</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -1856,10 +1856,10 @@
         <v>53</v>
       </c>
       <c r="D76">
-        <v>111.7</v>
+        <v>111</v>
       </c>
       <c r="E76">
-        <v>2566568</v>
+        <v>11520063</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -1890,10 +1890,10 @@
         <v>55</v>
       </c>
       <c r="D78">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E78">
-        <v>1340337</v>
+        <v>16118516</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -1927,7 +1927,7 @@
         <v>270</v>
       </c>
       <c r="E80">
-        <v>1108906</v>
+        <v>1105906</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -1941,10 +1941,10 @@
         <v>53</v>
       </c>
       <c r="D81">
-        <v>13090</v>
+        <v>12750</v>
       </c>
       <c r="E81">
-        <v>51000</v>
+        <v>151622</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -1978,7 +1978,7 @@
         <v>14850</v>
       </c>
       <c r="E83">
-        <v>68777</v>
+        <v>67877</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -2009,10 +2009,10 @@
         <v>53</v>
       </c>
       <c r="D85">
-        <v>11470</v>
+        <v>11440</v>
       </c>
       <c r="E85">
-        <v>28315</v>
+        <v>47002</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -2026,10 +2026,10 @@
         <v>55</v>
       </c>
       <c r="D86">
-        <v>27000</v>
+        <v>26990</v>
       </c>
       <c r="E86">
-        <v>63991</v>
+        <v>312354</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -2043,10 +2043,10 @@
         <v>53</v>
       </c>
       <c r="D87">
-        <v>99990</v>
+        <v>99980</v>
       </c>
       <c r="E87">
-        <v>10462</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2060,10 +2060,10 @@
         <v>54</v>
       </c>
       <c r="D88">
-        <v>115000</v>
+        <v>114800</v>
       </c>
       <c r="E88">
-        <v>666</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -2094,10 +2094,10 @@
         <v>53</v>
       </c>
       <c r="D90">
-        <v>44480</v>
+        <v>44000</v>
       </c>
       <c r="E90">
-        <v>2500</v>
+        <v>12773</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -2105,33 +2105,33 @@
         <v>34</v>
       </c>
       <c r="B91" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C91" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D91">
-        <v>38460</v>
+        <v>68380</v>
       </c>
       <c r="E91">
-        <v>3275</v>
+        <v>16088</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B92" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C92" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D92">
-        <v>68380</v>
+        <v>21000</v>
       </c>
       <c r="E92">
-        <v>16088</v>
+        <v>9220</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2139,16 +2139,16 @@
         <v>35</v>
       </c>
       <c r="B93" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C93" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D93">
-        <v>20990</v>
+        <v>29740</v>
       </c>
       <c r="E93">
-        <v>5921</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -2156,33 +2156,33 @@
         <v>35</v>
       </c>
       <c r="B94" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C94" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D94">
-        <v>29740</v>
+        <v>24390</v>
       </c>
       <c r="E94">
-        <v>10000</v>
+        <v>22649</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B95" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C95" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D95">
-        <v>24390</v>
+        <v>42270</v>
       </c>
       <c r="E95">
-        <v>22649</v>
+        <v>36322</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2190,16 +2190,16 @@
         <v>36</v>
       </c>
       <c r="B96" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C96" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D96">
-        <v>42270</v>
+        <v>69690</v>
       </c>
       <c r="E96">
-        <v>40037</v>
+        <v>5329</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2207,33 +2207,33 @@
         <v>36</v>
       </c>
       <c r="B97" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C97" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D97">
-        <v>69690</v>
+        <v>70390</v>
       </c>
       <c r="E97">
-        <v>5329</v>
+        <v>12966</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B98" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C98" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D98">
-        <v>70390</v>
+        <v>47990</v>
       </c>
       <c r="E98">
-        <v>12966</v>
+        <v>84098</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2241,16 +2241,16 @@
         <v>37</v>
       </c>
       <c r="B99" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C99" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D99">
-        <v>47990</v>
+        <v>87490</v>
       </c>
       <c r="E99">
-        <v>24639</v>
+        <v>25079</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -2258,33 +2258,33 @@
         <v>37</v>
       </c>
       <c r="B100" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C100" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D100">
-        <v>87490</v>
+        <v>75000</v>
       </c>
       <c r="E100">
-        <v>25079</v>
+        <v>31293</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B101" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C101" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D101">
-        <v>75000</v>
+        <v>39480</v>
       </c>
       <c r="E101">
-        <v>31293</v>
+        <v>2854</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -2292,16 +2292,16 @@
         <v>38</v>
       </c>
       <c r="B102" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C102" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D102">
-        <v>39580</v>
+        <v>46000</v>
       </c>
       <c r="E102">
-        <v>2756</v>
+        <v>3723</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2309,33 +2309,33 @@
         <v>38</v>
       </c>
       <c r="B103" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C103" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D103">
-        <v>46000</v>
+        <v>47330</v>
       </c>
       <c r="E103">
-        <v>3873</v>
+        <v>2574</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B104" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C104" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D104">
-        <v>47380</v>
+        <v>196.5</v>
       </c>
       <c r="E104">
-        <v>2574</v>
+        <v>6457301</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2343,16 +2343,16 @@
         <v>39</v>
       </c>
       <c r="B105" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C105" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D105">
-        <v>197.9</v>
+        <v>231</v>
       </c>
       <c r="E105">
-        <v>2539486</v>
+        <v>790100</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2360,16 +2360,16 @@
         <v>39</v>
       </c>
       <c r="B106" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C106" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D106">
-        <v>298.9</v>
+        <v>220</v>
       </c>
       <c r="E106">
-        <v>752229</v>
+        <v>4918864</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2377,50 +2377,50 @@
         <v>39</v>
       </c>
       <c r="B107" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C107" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D107">
-        <v>232.9</v>
+        <v>250</v>
       </c>
       <c r="E107">
-        <v>1973267</v>
+        <v>1255330</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B108" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C108" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D108">
-        <v>220</v>
+        <v>13350</v>
       </c>
       <c r="E108">
-        <v>4918864</v>
+        <v>126961</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B109" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C109" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D109">
-        <v>250</v>
+        <v>21530</v>
       </c>
       <c r="E109">
-        <v>1280500</v>
+        <v>39998</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -2428,50 +2428,50 @@
         <v>40</v>
       </c>
       <c r="B110" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C110" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D110">
-        <v>13470</v>
+        <v>18480</v>
       </c>
       <c r="E110">
-        <v>42284</v>
+        <v>105400</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B111" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C111" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D111">
-        <v>21570</v>
+        <v>80590</v>
       </c>
       <c r="E111">
-        <v>47998</v>
+        <v>462</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B112" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C112" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D112">
-        <v>18480</v>
+        <v>99900</v>
       </c>
       <c r="E112">
-        <v>105400</v>
+        <v>2895</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -2479,16 +2479,16 @@
         <v>41</v>
       </c>
       <c r="B113" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C113" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D113">
-        <v>80930</v>
+        <v>77300</v>
       </c>
       <c r="E113">
-        <v>3000</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -2496,50 +2496,50 @@
         <v>41</v>
       </c>
       <c r="B114" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C114" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D114">
-        <v>99900</v>
+        <v>115000</v>
       </c>
       <c r="E114">
-        <v>3095</v>
+        <v>2925</v>
       </c>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B115" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C115" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D115">
-        <v>77380</v>
+        <v>1820</v>
       </c>
       <c r="E115">
-        <v>2000</v>
+        <v>959714</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B116" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C116" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D116">
-        <v>115000</v>
+        <v>2660</v>
       </c>
       <c r="E116">
-        <v>2945</v>
+        <v>99985</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -2547,16 +2547,16 @@
         <v>42</v>
       </c>
       <c r="B117" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C117" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D117">
-        <v>1826</v>
+        <v>2748</v>
       </c>
       <c r="E117">
-        <v>459903</v>
+        <v>110952</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -2564,16 +2564,16 @@
         <v>42</v>
       </c>
       <c r="B118" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C118" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D118">
-        <v>2664</v>
+        <v>2388</v>
       </c>
       <c r="E118">
-        <v>400000</v>
+        <v>103369</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -2581,50 +2581,50 @@
         <v>42</v>
       </c>
       <c r="B119" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C119" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D119">
-        <v>2748</v>
+        <v>2850</v>
       </c>
       <c r="E119">
-        <v>178802</v>
+        <v>736038</v>
       </c>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B120" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C120" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D120">
-        <v>2388</v>
+        <v>28250</v>
       </c>
       <c r="E120">
-        <v>103369</v>
+        <v>244498</v>
       </c>
     </row>
     <row r="121" spans="1:5">
       <c r="A121" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B121" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C121" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D121">
-        <v>2850</v>
+        <v>35990</v>
       </c>
       <c r="E121">
-        <v>736038</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -2632,16 +2632,16 @@
         <v>43</v>
       </c>
       <c r="B122" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C122" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D122">
-        <v>28410</v>
+        <v>29010</v>
       </c>
       <c r="E122">
-        <v>14970</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -2649,16 +2649,16 @@
         <v>43</v>
       </c>
       <c r="B123" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C123" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D123">
-        <v>35990</v>
+        <v>31980</v>
       </c>
       <c r="E123">
-        <v>5000</v>
+        <v>8500</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -2666,50 +2666,50 @@
         <v>43</v>
       </c>
       <c r="B124" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C124" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D124">
-        <v>29010</v>
+        <v>39980</v>
       </c>
       <c r="E124">
-        <v>7200</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B125" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C125" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D125">
-        <v>31970</v>
+        <v>383.5</v>
       </c>
       <c r="E125">
-        <v>3000</v>
+        <v>10655809</v>
       </c>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B126" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C126" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D126">
-        <v>39980</v>
+        <v>994.1</v>
       </c>
       <c r="E126">
-        <v>7000</v>
+        <v>475005</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -2717,16 +2717,16 @@
         <v>44</v>
       </c>
       <c r="B127" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C127" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D127">
-        <v>388</v>
+        <v>579</v>
       </c>
       <c r="E127">
-        <v>1976423</v>
+        <v>240000</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -2734,50 +2734,50 @@
         <v>44</v>
       </c>
       <c r="B128" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C128" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D128">
-        <v>994.5</v>
+        <v>1000</v>
       </c>
       <c r="E128">
-        <v>991345</v>
+        <v>452469</v>
       </c>
     </row>
     <row r="129" spans="1:5">
       <c r="A129" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B129" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C129" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D129">
-        <v>590</v>
+        <v>2977</v>
       </c>
       <c r="E129">
-        <v>800000</v>
+        <v>57550</v>
       </c>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B130" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C130" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D130">
-        <v>1000</v>
+        <v>3949</v>
       </c>
       <c r="E130">
-        <v>452469</v>
+        <v>75195</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -2785,16 +2785,16 @@
         <v>45</v>
       </c>
       <c r="B131" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C131" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D131">
-        <v>2988</v>
+        <v>3500</v>
       </c>
       <c r="E131">
-        <v>132440</v>
+        <v>633739</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -2802,16 +2802,16 @@
         <v>45</v>
       </c>
       <c r="B132" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C132" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D132">
-        <v>3949</v>
+        <v>4995</v>
       </c>
       <c r="E132">
-        <v>96195</v>
+        <v>40750</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -2819,50 +2819,50 @@
         <v>45</v>
       </c>
       <c r="B133" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C133" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D133">
-        <v>3500</v>
+        <v>6284</v>
       </c>
       <c r="E133">
-        <v>646439</v>
+        <v>30273</v>
       </c>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B134" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C134" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D134">
-        <v>4995</v>
+        <v>6815</v>
       </c>
       <c r="E134">
-        <v>40750</v>
+        <v>265091</v>
       </c>
     </row>
     <row r="135" spans="1:5">
       <c r="A135" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B135" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C135" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D135">
-        <v>6284</v>
+        <v>8347</v>
       </c>
       <c r="E135">
-        <v>30273</v>
+        <v>12450</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -2870,16 +2870,16 @@
         <v>46</v>
       </c>
       <c r="B136" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C136" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D136">
-        <v>6832</v>
+        <v>7706</v>
       </c>
       <c r="E136">
-        <v>17617</v>
+        <v>75000</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -2887,50 +2887,50 @@
         <v>46</v>
       </c>
       <c r="B137" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C137" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D137">
-        <v>8347</v>
+        <v>10390</v>
       </c>
       <c r="E137">
-        <v>13502</v>
+        <v>19900</v>
       </c>
     </row>
     <row r="138" spans="1:5">
       <c r="A138" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B138" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C138" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D138">
-        <v>7706</v>
+        <v>1094</v>
       </c>
       <c r="E138">
-        <v>75000</v>
+        <v>81906</v>
       </c>
     </row>
     <row r="139" spans="1:5">
       <c r="A139" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B139" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C139" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D139">
-        <v>10390</v>
+        <v>1578</v>
       </c>
       <c r="E139">
-        <v>19900</v>
+        <v>288322</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -2938,16 +2938,16 @@
         <v>47</v>
       </c>
       <c r="B140" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C140" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D140">
-        <v>1095</v>
+        <v>1050</v>
       </c>
       <c r="E140">
-        <v>200000</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -2955,16 +2955,16 @@
         <v>47</v>
       </c>
       <c r="B141" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C141" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D141">
-        <v>1578</v>
+        <v>1399</v>
       </c>
       <c r="E141">
-        <v>299322</v>
+        <v>315814</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -2972,49 +2972,15 @@
         <v>47</v>
       </c>
       <c r="B142" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C142" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D142">
-        <v>1100</v>
+        <v>2000</v>
       </c>
       <c r="E142">
-        <v>374458</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5">
-      <c r="A143" t="s">
-        <v>47</v>
-      </c>
-      <c r="B143" t="s">
-        <v>51</v>
-      </c>
-      <c r="C143" t="s">
-        <v>56</v>
-      </c>
-      <c r="D143">
-        <v>1399</v>
-      </c>
-      <c r="E143">
-        <v>315814</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5">
-      <c r="A144" t="s">
-        <v>47</v>
-      </c>
-      <c r="B144" t="s">
-        <v>52</v>
-      </c>
-      <c r="C144" t="s">
-        <v>57</v>
-      </c>
-      <c r="D144">
-        <v>2000</v>
-      </c>
-      <c r="E144">
         <v>100000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
runtime improvements and basic frontend
</commit_message>
<xml_diff>
--- a/data/outputs/Market_Sell_Data.xlsx
+++ b/data/outputs/Market_Sell_Data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="66">
   <si>
     <t>Item</t>
   </si>
@@ -161,40 +161,46 @@
     <t>Fullerides</t>
   </si>
   <si>
-    <t>The Forge</t>
-  </si>
-  <si>
-    <t>Sinq Laison</t>
-  </si>
-  <si>
-    <t>Domain</t>
-  </si>
-  <si>
-    <t>Metropolis</t>
-  </si>
-  <si>
-    <t>Heimatar</t>
-  </si>
-  <si>
-    <t>Jita IV - Moon 4 - Caldari Navy Assembly Plant</t>
-  </si>
-  <si>
-    <t>Dodixie IX - Moon 20 - Federation Navy Assembly Plant</t>
-  </si>
-  <si>
-    <t>Amarr VIII (Oris) - Emperor Family Academy</t>
-  </si>
-  <si>
-    <t>Hek VIII - Moon 12 - Boundless Creation Factory</t>
-  </si>
-  <si>
-    <t>Rens VI - Moon 8 - Brutor Tribe Treasury</t>
-  </si>
-  <si>
-    <t>Dammalin VI - CBD Corporation Storage</t>
-  </si>
-  <si>
-    <t>Misaba V - Moon 3 - Zoar and Sons Factory</t>
+    <t>['The Forge']</t>
+  </si>
+  <si>
+    <t>['Sinq Laison']</t>
+  </si>
+  <si>
+    <t>['Domain']</t>
+  </si>
+  <si>
+    <t>['Metropolis']</t>
+  </si>
+  <si>
+    <t>['Heimatar']</t>
+  </si>
+  <si>
+    <t>['Jita IV - Moon 4 - Caldari Navy Assembly Plant']</t>
+  </si>
+  <si>
+    <t>['Dodixie IX - Moon 20 - Federation Navy Assembly Plant']</t>
+  </si>
+  <si>
+    <t>['Amarr VIII (Oris) - Emperor Family Academy']</t>
+  </si>
+  <si>
+    <t>['Hek VIII - Moon 12 - Boundless Creation Factory']</t>
+  </si>
+  <si>
+    <t>['Rens VI - Moon 8 - Brutor Tribe Treasury']</t>
+  </si>
+  <si>
+    <t>['Hadaugago II - Moon 1 - Republic Military School']</t>
+  </si>
+  <si>
+    <t>['Odebeinn V - Moon 5 - Kaalakiota Corporation Factory']</t>
+  </si>
+  <si>
+    <t>['Misaba V - Moon 3 - Zoar and Sons Factory']</t>
+  </si>
+  <si>
+    <t>['Josekorn VIII - CreoDron Factory']</t>
   </si>
   <si>
     <t>player_name</t>
@@ -206,7 +212,7 @@
     <t>Certh Finley</t>
   </si>
   <si>
-    <t>06/26/2023, 13:41:20</t>
+    <t>08/03/2023, 11:49:20</t>
   </si>
 </sst>
 </file>
@@ -564,7 +570,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E142"/>
+  <dimension ref="A1:E144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -598,10 +604,10 @@
         <v>53</v>
       </c>
       <c r="D2">
-        <v>133400</v>
+        <v>122900</v>
       </c>
       <c r="E2">
-        <v>4969</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -615,10 +621,10 @@
         <v>54</v>
       </c>
       <c r="D3">
-        <v>137900</v>
+        <v>147600</v>
       </c>
       <c r="E3">
-        <v>800</v>
+        <v>454</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -632,10 +638,10 @@
         <v>55</v>
       </c>
       <c r="D4">
-        <v>142500</v>
+        <v>244300</v>
       </c>
       <c r="E4">
-        <v>6495</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -649,10 +655,10 @@
         <v>56</v>
       </c>
       <c r="D5">
-        <v>149600</v>
+        <v>149000</v>
       </c>
       <c r="E5">
-        <v>422</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -666,7 +672,7 @@
         <v>57</v>
       </c>
       <c r="D6">
-        <v>400000</v>
+        <v>189000</v>
       </c>
       <c r="E6">
         <v>500</v>
@@ -683,10 +689,10 @@
         <v>53</v>
       </c>
       <c r="D7">
-        <v>39850</v>
+        <v>34300</v>
       </c>
       <c r="E7">
-        <v>54546</v>
+        <v>3136</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -703,7 +709,7 @@
         <v>41870</v>
       </c>
       <c r="E8">
-        <v>9392</v>
+        <v>8492</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -717,10 +723,10 @@
         <v>53</v>
       </c>
       <c r="D9">
-        <v>34480</v>
+        <v>47880</v>
       </c>
       <c r="E9">
-        <v>9571</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -728,33 +734,33 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D10">
-        <v>39990</v>
+        <v>90660</v>
       </c>
       <c r="E10">
-        <v>3631</v>
+        <v>9608</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D11">
-        <v>41970</v>
+        <v>55290</v>
       </c>
       <c r="E11">
-        <v>4644</v>
+        <v>25367</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -762,16 +768,16 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D12">
-        <v>58740</v>
+        <v>98790</v>
       </c>
       <c r="E12">
-        <v>24689</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -785,10 +791,10 @@
         <v>53</v>
       </c>
       <c r="D13">
-        <v>26640</v>
+        <v>27040</v>
       </c>
       <c r="E13">
-        <v>6680</v>
+        <v>4722</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -810,19 +816,19 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D15">
-        <v>33930</v>
+        <v>62570</v>
       </c>
       <c r="E15">
-        <v>5443</v>
+        <v>10739</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -830,16 +836,16 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D16">
-        <v>65310</v>
+        <v>61660</v>
       </c>
       <c r="E16">
-        <v>8000</v>
+        <v>4723</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -847,33 +853,33 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D17">
-        <v>97700</v>
+        <v>74870</v>
       </c>
       <c r="E17">
-        <v>5555</v>
+        <v>7877</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D18">
-        <v>74890</v>
+        <v>9980</v>
       </c>
       <c r="E18">
-        <v>5340</v>
+        <v>86102</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -881,16 +887,16 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D19">
-        <v>11490</v>
+        <v>21700</v>
       </c>
       <c r="E19">
-        <v>21250</v>
+        <v>22395</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -898,16 +904,16 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D20">
-        <v>27000</v>
+        <v>12300</v>
       </c>
       <c r="E20">
-        <v>25650</v>
+        <v>120580</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -915,33 +921,33 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D21">
-        <v>23320</v>
+        <v>12500</v>
       </c>
       <c r="E21">
-        <v>74245</v>
+        <v>29400</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D22">
-        <v>18000</v>
+        <v>154.5</v>
       </c>
       <c r="E22">
-        <v>20168</v>
+        <v>13016125</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -949,16 +955,16 @@
         <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D23">
-        <v>218.5</v>
+        <v>214</v>
       </c>
       <c r="E23">
-        <v>4233973</v>
+        <v>1899995</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -966,16 +972,16 @@
         <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D24">
-        <v>241.4</v>
+        <v>192.6</v>
       </c>
       <c r="E24">
-        <v>3432650</v>
+        <v>1687061</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -983,16 +989,16 @@
         <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D25">
-        <v>249</v>
+        <v>225.4</v>
       </c>
       <c r="E25">
-        <v>3615001</v>
+        <v>1960000</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1000,33 +1006,33 @@
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D26">
-        <v>250</v>
+        <v>296</v>
       </c>
       <c r="E26">
-        <v>2950000</v>
+        <v>1950000</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D27">
-        <v>296.5</v>
+        <v>20010</v>
       </c>
       <c r="E27">
-        <v>3638342</v>
+        <v>38916</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1034,50 +1040,50 @@
         <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D28">
-        <v>17100</v>
+        <v>37170</v>
       </c>
       <c r="E28">
-        <v>214722</v>
+        <v>49995</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D29">
-        <v>38590</v>
+        <v>125700</v>
       </c>
       <c r="E29">
-        <v>50000</v>
+        <v>550</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D30">
-        <v>22670</v>
+        <v>133500</v>
       </c>
       <c r="E30">
-        <v>59100</v>
+        <v>515</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1085,50 +1091,50 @@
         <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D31">
-        <v>179600</v>
+        <v>150000</v>
       </c>
       <c r="E31">
-        <v>9782</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D32">
-        <v>131900</v>
+        <v>45900</v>
       </c>
       <c r="E32">
-        <v>231</v>
+        <v>12311</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D33">
-        <v>104500</v>
+        <v>42890</v>
       </c>
       <c r="E33">
-        <v>2164</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1136,50 +1142,50 @@
         <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C34" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D34">
-        <v>42450</v>
+        <v>50730</v>
       </c>
       <c r="E34">
-        <v>19999</v>
+        <v>7471</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D35">
-        <v>55000</v>
+        <v>37340</v>
       </c>
       <c r="E35">
-        <v>2320</v>
+        <v>6959</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D36">
-        <v>51790</v>
+        <v>37880</v>
       </c>
       <c r="E36">
-        <v>2634</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1187,50 +1193,50 @@
         <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C37" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D37">
-        <v>37220</v>
+        <v>37500</v>
       </c>
       <c r="E37">
-        <v>70923</v>
+        <v>3071</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D38">
-        <v>38160</v>
+        <v>22870</v>
       </c>
       <c r="E38">
-        <v>4603</v>
+        <v>9732</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D39">
-        <v>38950</v>
+        <v>37750</v>
       </c>
       <c r="E39">
-        <v>6679</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1238,38 +1244,38 @@
         <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C40" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D40">
-        <v>19720</v>
+        <v>29600</v>
       </c>
       <c r="E40">
-        <v>101971</v>
+        <v>4914</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D41">
-        <v>37760</v>
+        <v>47000</v>
       </c>
       <c r="E41">
-        <v>4932</v>
+        <v>14278</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B42" t="s">
         <v>50</v>
@@ -1278,32 +1284,32 @@
         <v>55</v>
       </c>
       <c r="D42">
-        <v>32000</v>
+        <v>93000</v>
       </c>
       <c r="E42">
-        <v>7814</v>
+        <v>9505</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D43">
-        <v>58700</v>
+        <v>54750</v>
       </c>
       <c r="E43">
-        <v>5000</v>
+        <v>68638</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B44" t="s">
         <v>50</v>
@@ -1312,15 +1318,15 @@
         <v>55</v>
       </c>
       <c r="D44">
-        <v>47940</v>
+        <v>84990</v>
       </c>
       <c r="E44">
-        <v>10478</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B45" t="s">
         <v>48</v>
@@ -1329,27 +1335,27 @@
         <v>53</v>
       </c>
       <c r="D45">
-        <v>55670</v>
+        <v>9999</v>
       </c>
       <c r="E45">
-        <v>34609</v>
+        <v>64523</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D46">
-        <v>87870</v>
+        <v>17490</v>
       </c>
       <c r="E46">
-        <v>29960</v>
+        <v>25210</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1357,16 +1363,16 @@
         <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D47">
-        <v>11430</v>
+        <v>23950</v>
       </c>
       <c r="E47">
-        <v>21725</v>
+        <v>30100</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1374,33 +1380,33 @@
         <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C48" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D48">
-        <v>25950</v>
+        <v>11000</v>
       </c>
       <c r="E48">
-        <v>22000</v>
+        <v>27780</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B49" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D49">
-        <v>26870</v>
+        <v>147.4</v>
       </c>
       <c r="E49">
-        <v>163730</v>
+        <v>1470000</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1408,16 +1414,16 @@
         <v>21</v>
       </c>
       <c r="B50" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D50">
-        <v>169.5</v>
+        <v>187.9</v>
       </c>
       <c r="E50">
-        <v>3683907</v>
+        <v>998995</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1425,16 +1431,16 @@
         <v>21</v>
       </c>
       <c r="B51" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D51">
-        <v>213.6</v>
+        <v>263</v>
       </c>
       <c r="E51">
-        <v>1660805</v>
+        <v>921350</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1442,16 +1448,16 @@
         <v>21</v>
       </c>
       <c r="B52" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D52">
-        <v>209.8</v>
+        <v>221.2</v>
       </c>
       <c r="E52">
-        <v>2000000</v>
+        <v>3745356</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1459,33 +1465,33 @@
         <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C53" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D53">
-        <v>222.4</v>
+        <v>227.9</v>
       </c>
       <c r="E53">
-        <v>4990000</v>
+        <v>4055456</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B54" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C54" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D54">
-        <v>230.1</v>
+        <v>16290</v>
       </c>
       <c r="E54">
-        <v>997750</v>
+        <v>34332</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1493,33 +1499,33 @@
         <v>22</v>
       </c>
       <c r="B55" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C55" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D55">
-        <v>16550</v>
+        <v>38940</v>
       </c>
       <c r="E55">
-        <v>197452</v>
+        <v>38716</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B56" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C56" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D56">
-        <v>24970</v>
+        <v>41900</v>
       </c>
       <c r="E56">
-        <v>54000</v>
+        <v>4956</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1527,16 +1533,16 @@
         <v>23</v>
       </c>
       <c r="B57" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C57" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D57">
-        <v>40430</v>
+        <v>50000</v>
       </c>
       <c r="E57">
-        <v>5534</v>
+        <v>7127</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1544,38 +1550,38 @@
         <v>23</v>
       </c>
       <c r="B58" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C58" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D58">
-        <v>50000</v>
+        <v>48170</v>
       </c>
       <c r="E58">
-        <v>7639</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B59" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C59" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D59">
-        <v>48380</v>
+        <v>43910</v>
       </c>
       <c r="E59">
-        <v>4665</v>
+        <v>14182</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B60" t="s">
         <v>48</v>
@@ -1584,27 +1590,27 @@
         <v>53</v>
       </c>
       <c r="D60">
-        <v>45000</v>
+        <v>7598</v>
       </c>
       <c r="E60">
-        <v>20000</v>
+        <v>34011</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B61" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C61" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D61">
-        <v>59040</v>
+        <v>19870</v>
       </c>
       <c r="E61">
-        <v>30000</v>
+        <v>31997</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1612,16 +1618,16 @@
         <v>25</v>
       </c>
       <c r="B62" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C62" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D62">
-        <v>10450</v>
+        <v>26000</v>
       </c>
       <c r="E62">
-        <v>25000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1629,89 +1635,89 @@
         <v>25</v>
       </c>
       <c r="B63" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C63" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D63">
-        <v>19200</v>
+        <v>13800</v>
       </c>
       <c r="E63">
-        <v>61145</v>
+        <v>49840</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C64" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D64">
-        <v>17960</v>
+        <v>23920</v>
       </c>
       <c r="E64">
-        <v>88271</v>
+        <v>5023</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B65" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C65" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D65">
-        <v>19180</v>
+        <v>41150</v>
       </c>
       <c r="E65">
-        <v>20000</v>
+        <v>3528</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B66" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C66" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D66">
-        <v>19280</v>
+        <v>38970</v>
       </c>
       <c r="E66">
-        <v>9004</v>
+        <v>2842</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B67" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C67" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D67">
-        <v>20000</v>
+        <v>47350</v>
       </c>
       <c r="E67">
-        <v>5760</v>
+        <v>3374</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B68" t="s">
         <v>48</v>
@@ -1720,15 +1726,15 @@
         <v>53</v>
       </c>
       <c r="D68">
-        <v>38780</v>
+        <v>99780</v>
       </c>
       <c r="E68">
-        <v>22365</v>
+        <v>3365</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B69" t="s">
         <v>49</v>
@@ -1737,32 +1743,32 @@
         <v>54</v>
       </c>
       <c r="D69">
-        <v>41960</v>
+        <v>94780</v>
       </c>
       <c r="E69">
-        <v>1900</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B70" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C70" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D70">
-        <v>49240</v>
+        <v>95000</v>
       </c>
       <c r="E70">
-        <v>6917</v>
+        <v>494</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B71" t="s">
         <v>48</v>
@@ -1771,78 +1777,78 @@
         <v>53</v>
       </c>
       <c r="D71">
-        <v>98910</v>
+        <v>37320</v>
       </c>
       <c r="E71">
-        <v>6127</v>
+        <v>12550</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B72" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C72" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D72">
-        <v>94800</v>
+        <v>114.3</v>
       </c>
       <c r="E72">
-        <v>2364</v>
+        <v>2171271</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B73" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C73" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D73">
-        <v>95000</v>
+        <v>129.2</v>
       </c>
       <c r="E73">
-        <v>1624</v>
+        <v>995000</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B74" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C74" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D74">
-        <v>34470</v>
+        <v>139</v>
       </c>
       <c r="E74">
-        <v>14243</v>
+        <v>4512628</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B75" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C75" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D75">
-        <v>45830</v>
+        <v>100</v>
       </c>
       <c r="E75">
-        <v>6890</v>
+        <v>760000</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1850,174 +1856,174 @@
         <v>30</v>
       </c>
       <c r="B76" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C76" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D76">
-        <v>111</v>
+        <v>199</v>
       </c>
       <c r="E76">
-        <v>11520063</v>
+        <v>4132632</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B77" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D77">
-        <v>199.2</v>
+        <v>13300</v>
       </c>
       <c r="E77">
-        <v>872304</v>
+        <v>194191</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B78" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C78" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D78">
-        <v>172</v>
+        <v>24800</v>
       </c>
       <c r="E78">
-        <v>16118516</v>
+        <v>88760</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B79" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C79" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D79">
-        <v>180</v>
+        <v>14330</v>
       </c>
       <c r="E79">
-        <v>3000000</v>
+        <v>63675</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B80" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C80" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D80">
-        <v>270</v>
+        <v>9461</v>
       </c>
       <c r="E80">
-        <v>1105906</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B81" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C81" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D81">
-        <v>12750</v>
+        <v>13860</v>
       </c>
       <c r="E81">
-        <v>151622</v>
+        <v>20600</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B82" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C82" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D82">
-        <v>16860</v>
+        <v>14000</v>
       </c>
       <c r="E82">
-        <v>30000</v>
+        <v>86936</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B83" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C83" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D83">
-        <v>14850</v>
+        <v>12500</v>
       </c>
       <c r="E83">
-        <v>67877</v>
+        <v>27410</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B84" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C84" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D84">
-        <v>20000</v>
+        <v>124900</v>
       </c>
       <c r="E84">
-        <v>52900</v>
+        <v>7330</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B85" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C85" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D85">
-        <v>11440</v>
+        <v>125000</v>
       </c>
       <c r="E85">
-        <v>47002</v>
+        <v>945</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B86" t="s">
         <v>50</v>
@@ -2026,10 +2032,10 @@
         <v>55</v>
       </c>
       <c r="D86">
-        <v>26990</v>
+        <v>170000</v>
       </c>
       <c r="E86">
-        <v>312354</v>
+        <v>234</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -2037,16 +2043,16 @@
         <v>33</v>
       </c>
       <c r="B87" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C87" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D87">
-        <v>99980</v>
+        <v>589800</v>
       </c>
       <c r="E87">
-        <v>2136</v>
+        <v>501</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2054,33 +2060,33 @@
         <v>33</v>
       </c>
       <c r="B88" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C88" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D88">
-        <v>114800</v>
+        <v>122400</v>
       </c>
       <c r="E88">
-        <v>2000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B89" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C89" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D89">
-        <v>108100</v>
+        <v>43340</v>
       </c>
       <c r="E89">
-        <v>499</v>
+        <v>10500</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -2088,33 +2094,33 @@
         <v>34</v>
       </c>
       <c r="B90" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C90" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D90">
-        <v>44000</v>
+        <v>48930</v>
       </c>
       <c r="E90">
-        <v>12773</v>
+        <v>16088</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B91" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C91" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D91">
-        <v>68380</v>
+        <v>25390</v>
       </c>
       <c r="E91">
-        <v>16088</v>
+        <v>8238</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -2122,50 +2128,50 @@
         <v>35</v>
       </c>
       <c r="B92" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C92" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D92">
-        <v>21000</v>
+        <v>29740</v>
       </c>
       <c r="E92">
-        <v>9220</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B93" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C93" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D93">
-        <v>29740</v>
+        <v>53740</v>
       </c>
       <c r="E93">
-        <v>10000</v>
+        <v>8906</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B94" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C94" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D94">
-        <v>24390</v>
+        <v>69670</v>
       </c>
       <c r="E94">
-        <v>22649</v>
+        <v>5041</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2173,50 +2179,50 @@
         <v>36</v>
       </c>
       <c r="B95" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C95" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D95">
-        <v>42270</v>
+        <v>129700</v>
       </c>
       <c r="E95">
-        <v>36322</v>
+        <v>9824</v>
       </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B96" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C96" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D96">
-        <v>69690</v>
+        <v>52620</v>
       </c>
       <c r="E96">
-        <v>5329</v>
+        <v>48100</v>
       </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B97" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C97" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D97">
-        <v>70390</v>
+        <v>87490</v>
       </c>
       <c r="E97">
-        <v>12966</v>
+        <v>20607</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2224,50 +2230,50 @@
         <v>37</v>
       </c>
       <c r="B98" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C98" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D98">
-        <v>47990</v>
+        <v>68650</v>
       </c>
       <c r="E98">
-        <v>84098</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B99" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C99" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D99">
-        <v>87490</v>
+        <v>44860</v>
       </c>
       <c r="E99">
-        <v>25079</v>
+        <v>6964</v>
       </c>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B100" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C100" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D100">
-        <v>75000</v>
+        <v>46710</v>
       </c>
       <c r="E100">
-        <v>31293</v>
+        <v>3019</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -2275,50 +2281,50 @@
         <v>38</v>
       </c>
       <c r="B101" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C101" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D101">
-        <v>39480</v>
+        <v>69140</v>
       </c>
       <c r="E101">
-        <v>2854</v>
+        <v>9472</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B102" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C102" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D102">
-        <v>46000</v>
+        <v>139</v>
       </c>
       <c r="E102">
-        <v>3723</v>
+        <v>2400000</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B103" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C103" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D103">
-        <v>47330</v>
+        <v>199.9</v>
       </c>
       <c r="E103">
-        <v>2574</v>
+        <v>794949</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -2326,16 +2332,16 @@
         <v>39</v>
       </c>
       <c r="B104" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C104" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D104">
-        <v>196.5</v>
+        <v>148.1</v>
       </c>
       <c r="E104">
-        <v>6457301</v>
+        <v>1813836</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2343,16 +2349,16 @@
         <v>39</v>
       </c>
       <c r="B105" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C105" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D105">
-        <v>231</v>
+        <v>214.3</v>
       </c>
       <c r="E105">
-        <v>790100</v>
+        <v>1684000</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2360,33 +2366,33 @@
         <v>39</v>
       </c>
       <c r="B106" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C106" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D106">
-        <v>220</v>
+        <v>250.6</v>
       </c>
       <c r="E106">
-        <v>4918864</v>
+        <v>1722536</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B107" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C107" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D107">
-        <v>250</v>
+        <v>15370</v>
       </c>
       <c r="E107">
-        <v>1255330</v>
+        <v>76538</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2394,16 +2400,16 @@
         <v>40</v>
       </c>
       <c r="B108" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C108" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D108">
-        <v>13350</v>
+        <v>20250</v>
       </c>
       <c r="E108">
-        <v>126961</v>
+        <v>66500</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -2411,33 +2417,33 @@
         <v>40</v>
       </c>
       <c r="B109" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C109" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D109">
-        <v>21530</v>
+        <v>19530</v>
       </c>
       <c r="E109">
-        <v>39998</v>
+        <v>33893</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B110" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C110" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D110">
-        <v>18480</v>
+        <v>56800</v>
       </c>
       <c r="E110">
-        <v>105400</v>
+        <v>2241</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -2445,16 +2451,16 @@
         <v>41</v>
       </c>
       <c r="B111" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C111" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D111">
-        <v>80590</v>
+        <v>73970</v>
       </c>
       <c r="E111">
-        <v>462</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -2462,16 +2468,16 @@
         <v>41</v>
       </c>
       <c r="B112" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C112" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D112">
-        <v>99900</v>
+        <v>74400</v>
       </c>
       <c r="E112">
-        <v>2895</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -2479,16 +2485,16 @@
         <v>41</v>
       </c>
       <c r="B113" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C113" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D113">
-        <v>77300</v>
+        <v>79970</v>
       </c>
       <c r="E113">
-        <v>1168</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -2502,10 +2508,10 @@
         <v>57</v>
       </c>
       <c r="D114">
-        <v>115000</v>
+        <v>109700</v>
       </c>
       <c r="E114">
-        <v>2925</v>
+        <v>500</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -2519,10 +2525,10 @@
         <v>53</v>
       </c>
       <c r="D115">
-        <v>1820</v>
+        <v>1456</v>
       </c>
       <c r="E115">
-        <v>959714</v>
+        <v>51397</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -2536,10 +2542,10 @@
         <v>54</v>
       </c>
       <c r="D116">
-        <v>2660</v>
+        <v>1989</v>
       </c>
       <c r="E116">
-        <v>99985</v>
+        <v>230379</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -2553,10 +2559,10 @@
         <v>55</v>
       </c>
       <c r="D117">
-        <v>2748</v>
+        <v>1643</v>
       </c>
       <c r="E117">
-        <v>110952</v>
+        <v>102228</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -2570,10 +2576,10 @@
         <v>56</v>
       </c>
       <c r="D118">
-        <v>2388</v>
+        <v>2099</v>
       </c>
       <c r="E118">
-        <v>103369</v>
+        <v>151744</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -2587,10 +2593,10 @@
         <v>57</v>
       </c>
       <c r="D119">
-        <v>2850</v>
+        <v>1600</v>
       </c>
       <c r="E119">
-        <v>736038</v>
+        <v>75000</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -2604,10 +2610,10 @@
         <v>53</v>
       </c>
       <c r="D120">
-        <v>28250</v>
+        <v>34600</v>
       </c>
       <c r="E120">
-        <v>244498</v>
+        <v>91400</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -2621,10 +2627,10 @@
         <v>54</v>
       </c>
       <c r="D121">
-        <v>35990</v>
+        <v>33640</v>
       </c>
       <c r="E121">
-        <v>3800</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -2635,13 +2641,13 @@
         <v>50</v>
       </c>
       <c r="C122" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D122">
-        <v>29010</v>
+        <v>38880</v>
       </c>
       <c r="E122">
-        <v>7200</v>
+        <v>2839</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -2655,10 +2661,10 @@
         <v>56</v>
       </c>
       <c r="D123">
-        <v>31980</v>
+        <v>37980</v>
       </c>
       <c r="E123">
-        <v>8500</v>
+        <v>3157</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -2672,10 +2678,10 @@
         <v>57</v>
       </c>
       <c r="D124">
-        <v>39980</v>
+        <v>39970</v>
       </c>
       <c r="E124">
-        <v>7000</v>
+        <v>12100</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -2689,10 +2695,10 @@
         <v>53</v>
       </c>
       <c r="D125">
-        <v>383.5</v>
+        <v>286</v>
       </c>
       <c r="E125">
-        <v>10655809</v>
+        <v>9052591</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -2706,10 +2712,10 @@
         <v>54</v>
       </c>
       <c r="D126">
-        <v>994.1</v>
+        <v>430.8</v>
       </c>
       <c r="E126">
-        <v>475005</v>
+        <v>931295</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -2723,10 +2729,10 @@
         <v>55</v>
       </c>
       <c r="D127">
-        <v>579</v>
+        <v>425</v>
       </c>
       <c r="E127">
-        <v>240000</v>
+        <v>348000</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -2734,33 +2740,33 @@
         <v>44</v>
       </c>
       <c r="B128" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C128" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D128">
-        <v>1000</v>
+        <v>478.8</v>
       </c>
       <c r="E128">
-        <v>452469</v>
+        <v>893959</v>
       </c>
     </row>
     <row r="129" spans="1:5">
       <c r="A129" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B129" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C129" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D129">
-        <v>2977</v>
+        <v>799</v>
       </c>
       <c r="E129">
-        <v>57550</v>
+        <v>291012</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -2768,16 +2774,16 @@
         <v>45</v>
       </c>
       <c r="B130" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C130" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D130">
-        <v>3949</v>
+        <v>4015</v>
       </c>
       <c r="E130">
-        <v>75195</v>
+        <v>33488</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -2785,16 +2791,16 @@
         <v>45</v>
       </c>
       <c r="B131" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C131" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D131">
-        <v>3500</v>
+        <v>4499</v>
       </c>
       <c r="E131">
-        <v>633739</v>
+        <v>64217</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -2802,16 +2808,16 @@
         <v>45</v>
       </c>
       <c r="B132" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C132" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D132">
-        <v>4995</v>
+        <v>4355</v>
       </c>
       <c r="E132">
-        <v>40750</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -2819,33 +2825,33 @@
         <v>45</v>
       </c>
       <c r="B133" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C133" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D133">
-        <v>6284</v>
+        <v>4985</v>
       </c>
       <c r="E133">
-        <v>30273</v>
+        <v>98394</v>
       </c>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B134" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C134" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D134">
-        <v>6815</v>
+        <v>4999</v>
       </c>
       <c r="E134">
-        <v>265091</v>
+        <v>79185</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -2853,16 +2859,16 @@
         <v>46</v>
       </c>
       <c r="B135" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C135" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D135">
-        <v>8347</v>
+        <v>7433</v>
       </c>
       <c r="E135">
-        <v>12450</v>
+        <v>29988</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -2870,16 +2876,16 @@
         <v>46</v>
       </c>
       <c r="B136" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C136" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D136">
-        <v>7706</v>
+        <v>8487</v>
       </c>
       <c r="E136">
-        <v>75000</v>
+        <v>19580</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -2887,50 +2893,50 @@
         <v>46</v>
       </c>
       <c r="B137" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C137" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D137">
-        <v>10390</v>
+        <v>7706</v>
       </c>
       <c r="E137">
-        <v>19900</v>
+        <v>63799</v>
       </c>
     </row>
     <row r="138" spans="1:5">
       <c r="A138" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B138" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C138" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D138">
-        <v>1094</v>
+        <v>8297</v>
       </c>
       <c r="E138">
-        <v>81906</v>
+        <v>8440</v>
       </c>
     </row>
     <row r="139" spans="1:5">
       <c r="A139" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B139" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C139" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D139">
-        <v>1578</v>
+        <v>12980</v>
       </c>
       <c r="E139">
-        <v>288322</v>
+        <v>48703</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -2938,16 +2944,16 @@
         <v>47</v>
       </c>
       <c r="B140" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C140" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D140">
-        <v>1050</v>
+        <v>649.9</v>
       </c>
       <c r="E140">
-        <v>60000</v>
+        <v>1385736</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -2955,16 +2961,16 @@
         <v>47</v>
       </c>
       <c r="B141" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C141" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D141">
-        <v>1399</v>
+        <v>685</v>
       </c>
       <c r="E141">
-        <v>315814</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -2972,16 +2978,50 @@
         <v>47</v>
       </c>
       <c r="B142" t="s">
+        <v>50</v>
+      </c>
+      <c r="C142" t="s">
+        <v>55</v>
+      </c>
+      <c r="D142">
+        <v>760</v>
+      </c>
+      <c r="E142">
+        <v>47319</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" t="s">
+        <v>47</v>
+      </c>
+      <c r="B143" t="s">
+        <v>51</v>
+      </c>
+      <c r="C143" t="s">
+        <v>61</v>
+      </c>
+      <c r="D143">
+        <v>1120</v>
+      </c>
+      <c r="E143">
+        <v>600529</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" t="s">
+        <v>47</v>
+      </c>
+      <c r="B144" t="s">
         <v>52</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C144" t="s">
         <v>57</v>
       </c>
-      <c r="D142">
-        <v>2000</v>
-      </c>
-      <c r="E142">
-        <v>100000</v>
+      <c r="D144">
+        <v>1399</v>
+      </c>
+      <c r="E144">
+        <v>108892</v>
       </c>
     </row>
   </sheetData>
@@ -2999,18 +3039,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>